<commit_message>
Created 10-bit HV Pot, Updated libraries, Updated IR sensor design
</commit_message>
<xml_diff>
--- a/IR Sensor/IRSensorCalcs.xlsx
+++ b/IR Sensor/IRSensorCalcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="16275" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="16275" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EmitterLED" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -180,12 +180,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,7 +492,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,17 +715,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">

</xml_diff>

<commit_message>
updating theremin related files
</commit_message>
<xml_diff>
--- a/IR Sensor/IRSensorCalcs.xlsx
+++ b/IR Sensor/IRSensorCalcs.xlsx
@@ -492,7 +492,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -564,7 +564,7 @@
       </c>
       <c r="B7">
         <f>B6-B4</f>
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -579,7 +579,7 @@
       </c>
       <c r="B8">
         <f>B7/B2</f>
-        <v>35</v>
+        <v>32.999999999999993</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -611,7 +611,7 @@
       </c>
       <c r="B12" s="2">
         <f>B7/B10</f>
-        <v>8.5365853658536592E-2</v>
+        <v>8.0487804878048783E-2</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -623,7 +623,7 @@
       </c>
       <c r="B13" s="2">
         <f>B12*B12*B10</f>
-        <v>0.29878048780487809</v>
+        <v>0.26560975609756099</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -635,7 +635,7 @@
       </c>
       <c r="B14" s="2">
         <f>B13/2</f>
-        <v>0.14939024390243905</v>
+        <v>0.13280487804878049</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -658,7 +658,7 @@
       </c>
       <c r="B16" s="2">
         <f>B14/B15</f>
-        <v>0.59756097560975618</v>
+        <v>0.53121951219512198</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -670,7 +670,7 @@
       </c>
       <c r="B18">
         <f>B12*B4</f>
-        <v>0.12804878048780488</v>
+        <v>0.13682926829268294</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -682,7 +682,7 @@
       </c>
       <c r="B19" s="2">
         <f>B18/B3</f>
-        <v>0.71138211382113825</v>
+        <v>0.72015404364569968</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -698,7 +698,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>